<commit_message>
Removing additional sheets from InputData excel files
</commit_message>
<xml_diff>
--- a/ExampleFolder/InputData/v_example/Country_Concordance_Full.xlsx
+++ b/ExampleFolder/InputData/v_example/Country_Concordance_Full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\Fellowship 1960-2015 PFU database\InputData\v1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\CL-PFU-JOSS-Paper\ExampleFolder\InputData\v_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C178976A-62CD-47F8-A9FE-4FE67E196228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9B8724-E335-42F5-9491-0C246AA636F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1620" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country_concordance_table" sheetId="1" r:id="rId1"/>
@@ -2765,7 +2765,7 @@
   <dimension ref="A1:H325"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>

</xml_diff>